<commit_message>
Added in GrimReaper skills doc 6 new skills.
</commit_message>
<xml_diff>
--- a/GameDesign/Class/6-GrimReaper/Documentation/GrimReaperSkills.xlsx
+++ b/GameDesign/Class/6-GrimReaper/Documentation/GrimReaperSkills.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17726"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Client\Desktop\My_Dev\BattleForVoxturia\GameDesign\Class\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Client\Desktop\My_Dev\BattleForVoxturia\GameDesign\Class\6-GrimReaper\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843" activeTab="5"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
-    <sheet name="Feuil1 (2)" sheetId="2" r:id="rId2"/>
-    <sheet name="Feuil1 (3)" sheetId="3" r:id="rId3"/>
-    <sheet name="Feuil1 (4)" sheetId="4" r:id="rId4"/>
-    <sheet name="Feuil1 (5)" sheetId="5" r:id="rId5"/>
-    <sheet name="Feuil1 (6)" sheetId="6" r:id="rId6"/>
+    <sheet name="1-ProtectiveWings" sheetId="1" r:id="rId1"/>
+    <sheet name="2-BlackMist" sheetId="2" r:id="rId2"/>
+    <sheet name="3-VitalDrain" sheetId="3" r:id="rId3"/>
+    <sheet name="4-MorbidReanimation" sheetId="4" r:id="rId4"/>
+    <sheet name="5-AssaultOfRavens" sheetId="5" r:id="rId5"/>
+    <sheet name="6-TombStone" sheetId="6" r:id="rId6"/>
     <sheet name="Feuil1 (7)" sheetId="7" r:id="rId7"/>
     <sheet name="Feuil1 (8)" sheetId="8" r:id="rId8"/>
     <sheet name="Feuil1 (9)" sheetId="9" r:id="rId9"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="74">
   <si>
     <t>[[AP: 0 ]]</t>
   </si>
@@ -90,6 +90,171 @@
   </si>
   <si>
     <t>[[Number of turns between two casts: -  ]]</t>
+  </si>
+  <si>
+    <t>Protective Wings</t>
+  </si>
+  <si>
+    <t>[[AP: 6 ]]</t>
+  </si>
+  <si>
+    <t>[[MP: 2 ]]</t>
+  </si>
+  <si>
+    <t>[[Range: 0 ]]</t>
+  </si>
+  <si>
+    <t>[[Modifiable range: No ]]</t>
+  </si>
+  <si>
+    <t>[[Number of turns between two casts: 6 ]]</t>
+  </si>
+  <si>
+    <t>[[Max effect accumulation: 1 ]]</t>
+  </si>
+  <si>
+    <t>[[Area of effect: - Single cell]]</t>
+  </si>
+  <si>
+    <t>[[Invulnerable]] (1 turn)</t>
+  </si>
+  <si>
+    <t>[[Unmovable]]   (1 turn)</t>
+  </si>
+  <si>
+    <t>Automatically end turn.</t>
+  </si>
+  <si>
+    <t>Black Mist</t>
+  </si>
+  <si>
+    <t>The caster become invulnerable and unmovable.</t>
+  </si>
+  <si>
+    <t>[[Reduce range by 100]] (2 turns)</t>
+  </si>
+  <si>
+    <t>[[AP: 5 ]]</t>
+  </si>
+  <si>
+    <t>[[MP: 1 ]]</t>
+  </si>
+  <si>
+    <t>[[Number of turns between two casts: 7 ]]</t>
+  </si>
+  <si>
+    <t>Every entity except the caster loose all the range.</t>
+  </si>
+  <si>
+    <t>[[Area of effect: - Every entity except the caster ]]</t>
+  </si>
+  <si>
+    <t>Vital Drain</t>
+  </si>
+  <si>
+    <t>Stealth Dark-type health.                                                                More effective on allies player</t>
+  </si>
+  <si>
+    <t>[[AP: 4 ]]</t>
+  </si>
+  <si>
+    <t>[[Range: 1-3 ]]</t>
+  </si>
+  <si>
+    <t>[[Modifiable range: Yes ]]</t>
+  </si>
+  <si>
+    <t>[[Range: 1-2 ]]</t>
+  </si>
+  <si>
+    <t>[[Line of sight: No ]]</t>
+  </si>
+  <si>
+    <t>[[Cast in straight line: No ]]</t>
+  </si>
+  <si>
+    <t>[[Number of casts per turn: 2 ]]</t>
+  </si>
+  <si>
+    <t>[[Number of cast per turn per target: 1 ]]</t>
+  </si>
+  <si>
+    <t>On allie:     [[Damage:  75-80 dark stealth]]</t>
+  </si>
+  <si>
+    <t>On enemy: [[Damage:  35-40 dark stealth]]</t>
+  </si>
+  <si>
+    <t>Morbid Reanimation</t>
+  </si>
+  <si>
+    <t>[[Line of sight: Yes ]]</t>
+  </si>
+  <si>
+    <t>[[Cast in straight line: Yes ]]</t>
+  </si>
+  <si>
+    <t>[[Number of turns between two casts: 2 ]]</t>
+  </si>
+  <si>
+    <t>Effect name: ''Reanimated''.</t>
+  </si>
+  <si>
+    <t>Effect name: ''Zombification''.</t>
+  </si>
+  <si>
+    <t>Target: Reanimate whit the ''Zombification'' effect. (00 turns)</t>
+  </si>
+  <si>
+    <t>Reanimate an K/O entity.                                                                      Can't be reanimated a second time.                                                               The reanimated entity take damage from healing but get healed from poison.                                                                                      The target must be K/O.</t>
+  </si>
+  <si>
+    <t>Target: [[-2 AP, -2 MP, -2 Range, -100% Light resistance]] (00 turns)</t>
+  </si>
+  <si>
+    <t>Caster: [[Reduce max HP by 10%]] (00 turns)</t>
+  </si>
+  <si>
+    <t>Target: [[HP set to 60% of max HP]]</t>
+  </si>
+  <si>
+    <t>Assault Of Ravens</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[[Area of effect: - Straight line of cells ]] (Modular area) </t>
+  </si>
+  <si>
+    <t>Inflicts Air-type damage in a modular area of effect.                        All the cells between the targetted cell and the caster are part of the area of effect.</t>
+  </si>
+  <si>
+    <t>[[AP: 3 ]]</t>
+  </si>
+  <si>
+    <t>[[Range: 1-4 ]]</t>
+  </si>
+  <si>
+    <t>[[Damage: 25-50 air ]]</t>
+  </si>
+  <si>
+    <t>Tomb Stone</t>
+  </si>
+  <si>
+    <t>[[AP: 2 ]]</t>
+  </si>
+  <si>
+    <t>[[Number of casts per turn: 1 ]]</t>
+  </si>
+  <si>
+    <t>[[Area of effect: - Single cell ]]</t>
+  </si>
+  <si>
+    <t>[[Damage:  15-20 earth ]]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inflicts Earth-type damage on entity.                                                 OR                                                                                                    Summons an unmovable Tomb Stone on an empty cell.                     </t>
+  </si>
+  <si>
+    <t>Summons a ''Pillar'' [[20% summoner HP, 0 AP, 0 MP, 20% earth resistence, 15% fire resistence, -30% water resistence, 10% air resistence, -50% light resistence, 50% dark resistence]]</t>
   </si>
 </sst>
 </file>
@@ -155,7 +320,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -172,11 +337,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -199,6 +379,19 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -514,10 +707,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D33"/>
+  <dimension ref="B2:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -537,7 +730,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -549,66 +742,64 @@
     <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="2" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
-      <c r="C6" s="9" t="s">
-        <v>14</v>
-      </c>
+      <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="C7" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
       <c r="C9" s="3" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
-      <c r="C10" s="3" t="s">
-        <v>2</v>
-      </c>
+      <c r="C10" s="3"/>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
-      <c r="C11" s="3"/>
+      <c r="C11" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
-      <c r="C12" s="3" t="s">
-        <v>4</v>
-      </c>
+      <c r="C12" s="3"/>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
       <c r="C13" s="3" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="3" t="s">
-        <v>3</v>
+      <c r="C14" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="D14" s="1"/>
     </row>
@@ -620,108 +811,68 @@
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
       <c r="C16" s="3" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="1"/>
-      <c r="C17" s="7" t="s">
-        <v>7</v>
-      </c>
+      <c r="C17" s="1"/>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B18" s="1"/>
-      <c r="C18" s="3"/>
+      <c r="C18" s="11" t="s">
+        <v>27</v>
+      </c>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B19" s="1"/>
-      <c r="C19" s="3" t="s">
-        <v>5</v>
+      <c r="C19" s="11" t="s">
+        <v>28</v>
       </c>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B20" s="1"/>
-      <c r="C20" s="3" t="s">
-        <v>6</v>
+      <c r="C20" s="11" t="s">
+        <v>29</v>
       </c>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
-      <c r="C21" s="3"/>
+      <c r="C21" s="1"/>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B22" s="1"/>
-      <c r="C22" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D22" s="1"/>
-    </row>
+    <row r="22" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B24" s="1"/>
-      <c r="C24" s="3" t="s">
-        <v>11</v>
+      <c r="C24" s="5" t="s">
+        <v>10</v>
       </c>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
-      <c r="C25" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="C25" s="1"/>
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
+      <c r="C26" s="10"/>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B29" s="1"/>
-      <c r="C29" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B31" s="1"/>
-      <c r="C31" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B32" s="1"/>
-      <c r="C32" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="6"/>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -948,10 +1099,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D33"/>
+  <dimension ref="B2:D24"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -971,7 +1122,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -983,179 +1134,116 @@
     <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="2" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
-      <c r="C6" s="9" t="s">
-        <v>14</v>
-      </c>
+      <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="C7" s="3" t="s">
+        <v>33</v>
+      </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
       <c r="C9" s="3" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
-      <c r="C10" s="3" t="s">
-        <v>2</v>
-      </c>
+      <c r="C10" s="3"/>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
-      <c r="C11" s="3"/>
+      <c r="C11" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
-      <c r="C12" s="3" t="s">
-        <v>4</v>
-      </c>
+      <c r="C12" s="3"/>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
       <c r="C13" s="3" t="s">
-        <v>8</v>
+        <v>35</v>
       </c>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="C14" s="3"/>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
-      <c r="C15" s="3"/>
+      <c r="C15" s="3" t="s">
+        <v>37</v>
+      </c>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
-      <c r="C16" s="3" t="s">
-        <v>18</v>
-      </c>
+      <c r="C16" s="1"/>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
-      <c r="C17" s="7" t="s">
-        <v>7</v>
+      <c r="C17" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
-      <c r="C18" s="3"/>
+      <c r="C18" s="1"/>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B19" s="1"/>
-      <c r="C19" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
-      <c r="C20" s="3" t="s">
-        <v>6</v>
-      </c>
+      <c r="C20" s="1"/>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B21" s="1"/>
-      <c r="C21" s="3"/>
+      <c r="C21" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
-      <c r="C22" s="3" t="s">
-        <v>9</v>
-      </c>
+      <c r="C22" s="1"/>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
+      <c r="C23" s="10"/>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
-      <c r="C24" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D24" s="1"/>
-    </row>
-    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B25" s="1"/>
-      <c r="C25" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D25" s="1"/>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-    </row>
-    <row r="27" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B29" s="1"/>
-      <c r="C29" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B31" s="1"/>
-      <c r="C31" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B32" s="1"/>
-      <c r="C32" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="6"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1165,10 +1253,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D33"/>
+  <dimension ref="B2:D27"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1188,7 +1276,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1197,182 +1285,140 @@
       <c r="C4" s="4"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:4" ht="39" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
-      <c r="C5" s="2" t="s">
-        <v>13</v>
+      <c r="C5" s="12" t="s">
+        <v>39</v>
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
-      <c r="C6" s="9" t="s">
-        <v>14</v>
-      </c>
+      <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="C7" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
-      <c r="C9" s="3" t="s">
-        <v>1</v>
-      </c>
+      <c r="C9" s="3"/>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="3" t="s">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
-      <c r="C11" s="3"/>
+      <c r="C11" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>4</v>
+        <v>45</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
-      <c r="C13" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="C13" s="3"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
       <c r="C14" s="3" t="s">
-        <v>3</v>
+        <v>46</v>
       </c>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
-      <c r="C15" s="3"/>
+      <c r="C15" s="3" t="s">
+        <v>47</v>
+      </c>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
-      <c r="C16" s="3" t="s">
-        <v>18</v>
-      </c>
+      <c r="C16" s="3"/>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
-      <c r="C17" s="7" t="s">
-        <v>7</v>
+      <c r="C17" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="1"/>
-      <c r="C18" s="3"/>
+      <c r="C18" s="1"/>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B19" s="1"/>
-      <c r="C19" s="3" t="s">
-        <v>5</v>
+      <c r="C19" s="11" t="s">
+        <v>49</v>
       </c>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B20" s="1"/>
-      <c r="C20" s="3" t="s">
-        <v>6</v>
+      <c r="C20" s="11" t="s">
+        <v>48</v>
       </c>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
-      <c r="C21" s="3"/>
+      <c r="C21" s="1"/>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B22" s="1"/>
-      <c r="C22" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D22" s="1"/>
-    </row>
+    <row r="22" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B24" s="1"/>
-      <c r="C24" s="3" t="s">
-        <v>11</v>
+      <c r="C24" s="5" t="s">
+        <v>10</v>
       </c>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
-      <c r="C25" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="C25" s="1"/>
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
+      <c r="C26" s="10"/>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B29" s="1"/>
-      <c r="C29" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B31" s="1"/>
-      <c r="C31" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B32" s="1"/>
-      <c r="C32" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="6"/>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1382,10 +1428,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D33"/>
+  <dimension ref="B2:D30"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1405,7 +1451,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1414,119 +1460,119 @@
       <c r="C4" s="4"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:4" ht="97.5" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
-      <c r="C5" s="2" t="s">
-        <v>13</v>
+      <c r="C5" s="14" t="s">
+        <v>57</v>
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
-      <c r="C6" s="9" t="s">
-        <v>14</v>
-      </c>
+      <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="C7" s="3" t="s">
+        <v>33</v>
+      </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
       <c r="C9" s="3" t="s">
-        <v>1</v>
+        <v>43</v>
       </c>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
-      <c r="C10" s="3" t="s">
-        <v>2</v>
-      </c>
+      <c r="C10" s="3"/>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
-      <c r="C11" s="3"/>
+      <c r="C11" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>4</v>
+        <v>51</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
       <c r="C13" s="3" t="s">
-        <v>8</v>
+        <v>52</v>
       </c>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="C14" s="3"/>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
-      <c r="C15" s="3"/>
+      <c r="C15" s="3" t="s">
+        <v>53</v>
+      </c>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
-      <c r="C16" s="3" t="s">
-        <v>18</v>
-      </c>
+      <c r="C16" s="3"/>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
-      <c r="C17" s="7" t="s">
-        <v>7</v>
+      <c r="C17" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="1"/>
-      <c r="C18" s="3"/>
+      <c r="C18" s="1"/>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B19" s="1"/>
-      <c r="C19" s="3" t="s">
-        <v>5</v>
+      <c r="C19" s="11" t="s">
+        <v>56</v>
       </c>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B20" s="1"/>
-      <c r="C20" s="3" t="s">
-        <v>6</v>
+      <c r="C20" s="11" t="s">
+        <v>58</v>
       </c>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B21" s="1"/>
-      <c r="C21" s="3"/>
+      <c r="C21" s="11" t="s">
+        <v>60</v>
+      </c>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B22" s="1"/>
-      <c r="C22" s="3" t="s">
-        <v>9</v>
+      <c r="C22" s="11" t="s">
+        <v>59</v>
       </c>
       <c r="D22" s="1"/>
     </row>
@@ -1535,61 +1581,42 @@
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B24" s="1"/>
-      <c r="C24" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D24" s="1"/>
-    </row>
-    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
-      <c r="C25" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="C25" s="1"/>
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
+      <c r="C26" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+    </row>
+    <row r="28" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
+      <c r="C28" s="13" t="s">
+        <v>54</v>
+      </c>
       <c r="D28" s="1"/>
     </row>
-    <row r="29" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="29" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B29" s="1"/>
-      <c r="C29" s="5" t="s">
-        <v>10</v>
+      <c r="C29" s="13" t="s">
+        <v>55</v>
       </c>
       <c r="D29" s="1"/>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B31" s="1"/>
-      <c r="C31" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B32" s="1"/>
-      <c r="C32" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="6"/>
+      <c r="D30" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1599,10 +1626,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D33"/>
+  <dimension ref="B2:D26"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1622,7 +1649,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>15</v>
+        <v>61</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1631,182 +1658,133 @@
       <c r="C4" s="4"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:4" ht="58.5" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
-      <c r="C5" s="2" t="s">
-        <v>13</v>
+      <c r="C5" s="14" t="s">
+        <v>63</v>
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
-      <c r="C6" s="9" t="s">
-        <v>14</v>
-      </c>
+      <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="C7" s="3" t="s">
+        <v>64</v>
+      </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
       <c r="C9" s="3" t="s">
-        <v>1</v>
+        <v>41</v>
       </c>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
-      <c r="C10" s="3" t="s">
-        <v>2</v>
-      </c>
+      <c r="C10" s="3"/>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
-      <c r="C11" s="3"/>
+      <c r="C11" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>4</v>
+        <v>44</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
       <c r="C13" s="3" t="s">
-        <v>8</v>
+        <v>52</v>
       </c>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="C14" s="3"/>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
-      <c r="C15" s="3"/>
+      <c r="C15" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
-      <c r="C16" s="3" t="s">
-        <v>18</v>
-      </c>
+      <c r="C16" s="3"/>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
-      <c r="C17" s="7" t="s">
-        <v>7</v>
+      <c r="C17" s="3" t="s">
+        <v>62</v>
       </c>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
-      <c r="C18" s="3"/>
+      <c r="C18" s="1"/>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
       <c r="C19" s="3" t="s">
-        <v>5</v>
+        <v>66</v>
       </c>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
-      <c r="C20" s="3" t="s">
-        <v>6</v>
-      </c>
+      <c r="C20" s="1"/>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B21" s="1"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
-      <c r="C22" s="3" t="s">
-        <v>9</v>
-      </c>
+      <c r="C22" s="1"/>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
+      <c r="C23" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
-      <c r="C24" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="C24" s="1"/>
       <c r="D24" s="1"/>
     </row>
     <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B25" s="1"/>
-      <c r="C25" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="C25" s="10"/>
       <c r="D25" s="1"/>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-    </row>
-    <row r="27" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B29" s="1"/>
-      <c r="C29" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B31" s="1"/>
-      <c r="C31" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B32" s="1"/>
-      <c r="C32" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="6"/>
+      <c r="D26" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1816,10 +1794,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D33"/>
+  <dimension ref="B2:D26"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1839,7 +1817,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>15</v>
+        <v>67</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1848,69 +1826,67 @@
       <c r="C4" s="4"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:4" ht="58.5" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
-      <c r="C5" s="2" t="s">
-        <v>13</v>
+      <c r="C5" s="14" t="s">
+        <v>72</v>
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
-      <c r="C6" s="9" t="s">
-        <v>14</v>
-      </c>
+      <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="C7" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
-      <c r="C9" s="3" t="s">
-        <v>1</v>
-      </c>
+      <c r="C9" s="3"/>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="3" t="s">
-        <v>2</v>
+        <v>42</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
-      <c r="C11" s="3"/>
+      <c r="C11" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>4</v>
+        <v>52</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
-      <c r="C13" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="C13" s="3"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
       <c r="C14" s="3" t="s">
-        <v>3</v>
+        <v>69</v>
       </c>
       <c r="D14" s="1"/>
     </row>
@@ -1922,108 +1898,61 @@
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
       <c r="C16" s="3" t="s">
-        <v>18</v>
+        <v>70</v>
       </c>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="1"/>
-      <c r="C17" s="7" t="s">
-        <v>7</v>
-      </c>
+      <c r="C17" s="1"/>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B18" s="1"/>
-      <c r="C18" s="3"/>
+      <c r="C18" s="11" t="s">
+        <v>71</v>
+      </c>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:4" ht="59.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B19" s="1"/>
-      <c r="C19" s="3" t="s">
-        <v>5</v>
+      <c r="C19" s="15" t="s">
+        <v>73</v>
       </c>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
-      <c r="C20" s="3" t="s">
-        <v>6</v>
-      </c>
+      <c r="C20" s="1"/>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B21" s="1"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
-      <c r="C22" s="3" t="s">
-        <v>9</v>
-      </c>
+      <c r="C22" s="1"/>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
+      <c r="C23" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
-      <c r="C24" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="C24" s="1"/>
       <c r="D24" s="1"/>
     </row>
     <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B25" s="1"/>
-      <c r="C25" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="C25" s="10"/>
       <c r="D25" s="1"/>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-    </row>
-    <row r="27" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B29" s="1"/>
-      <c r="C29" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B31" s="1"/>
-      <c r="C31" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B32" s="1"/>
-      <c r="C32" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="6"/>
+      <c r="D26" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added in GrimReaper skills doc 2 new skills. Also added some interesting resource for map view and sprite editor.
</commit_message>
<xml_diff>
--- a/GameDesign/Class/6-GrimReaper/Documentation/GrimReaperSkills.xlsx
+++ b/GameDesign/Class/6-GrimReaper/Documentation/GrimReaperSkills.xlsx
@@ -9,17 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843" firstSheet="4" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="1-ProtectiveWings" sheetId="1" r:id="rId1"/>
     <sheet name="2-BlackMist" sheetId="2" r:id="rId2"/>
     <sheet name="3-VitalDrain" sheetId="3" r:id="rId3"/>
     <sheet name="4-MorbidReanimation" sheetId="4" r:id="rId4"/>
-    <sheet name="5-AssaultOfRavens" sheetId="5" r:id="rId5"/>
+    <sheet name="5-RavensAssault" sheetId="5" r:id="rId5"/>
     <sheet name="6-TombStone" sheetId="6" r:id="rId6"/>
-    <sheet name="Feuil1 (7)" sheetId="7" r:id="rId7"/>
-    <sheet name="Feuil1 (8)" sheetId="8" r:id="rId8"/>
+    <sheet name="7-MaleficAura" sheetId="7" r:id="rId7"/>
+    <sheet name="8-ObscureSoaring" sheetId="8" r:id="rId8"/>
     <sheet name="Feuil1 (9)" sheetId="9" r:id="rId9"/>
     <sheet name="Feuil1 (10)" sheetId="10" r:id="rId10"/>
   </sheets>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="86">
   <si>
     <t>[[AP: 0 ]]</t>
   </si>
@@ -218,9 +218,6 @@
     <t>Target: [[HP set to 60% of max HP]]</t>
   </si>
   <si>
-    <t>Assault Of Ravens</t>
-  </si>
-  <si>
     <t xml:space="preserve">[[Area of effect: - Straight line of cells ]] (Modular area) </t>
   </si>
   <si>
@@ -255,6 +252,45 @@
   </si>
   <si>
     <t>Summons a ''Pillar'' [[20% summoner HP, 0 AP, 0 MP, 20% earth resistence, 15% fire resistence, -30% water resistence, 10% air resistence, -50% light resistence, 50% dark resistence]]</t>
+  </si>
+  <si>
+    <t>[[Area of effect: - Cross of 1 cell]]</t>
+  </si>
+  <si>
+    <t>Malefic Aura</t>
+  </si>
+  <si>
+    <t>[[Number of turns between two casts: 4 ]]</t>
+  </si>
+  <si>
+    <t>[[Boost damage dealt by 50%]] (1 turn)</t>
+  </si>
+  <si>
+    <t>[[Return 25% of damage dealt in Dark-type damage ]] (1 turn)</t>
+  </si>
+  <si>
+    <t>Effect name: ''Power''.</t>
+  </si>
+  <si>
+    <t>Effect name: ''Self Consumption''.</t>
+  </si>
+  <si>
+    <t>Boost the power of the caster and the entities around him.               The damage dealt are greater, but part of those damage are also taken by the holders of that aura.</t>
+  </si>
+  <si>
+    <t>Obscure Soaring</t>
+  </si>
+  <si>
+    <t>Ravens Assault</t>
+  </si>
+  <si>
+    <t>[[Number of turns between two casts: 2  ]]</t>
+  </si>
+  <si>
+    <t>Teleports to the targeted cell.</t>
+  </si>
+  <si>
+    <t>Teleport the caster at the targeted cell.</t>
   </si>
 </sst>
 </file>
@@ -1626,6 +1662,167 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:D25"/>
+  <sheetViews>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="2.85546875" customWidth="1"/>
+    <col min="3" max="3" width="85.7109375" customWidth="1"/>
+    <col min="4" max="6" width="2.85546875" customWidth="1"/>
+    <col min="7" max="7" width="78.5703125" customWidth="1"/>
+    <col min="8" max="8" width="2.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="1"/>
+      <c r="C3" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B4" s="1"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="2:4" ht="58.5" x14ac:dyDescent="0.25">
+      <c r="B5" s="1"/>
+      <c r="C5" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B7" s="1"/>
+      <c r="C7" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B8" s="1"/>
+      <c r="C8" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B9" s="1"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B10" s="1"/>
+      <c r="C10" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B11" s="1"/>
+      <c r="C11" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B12" s="1"/>
+      <c r="C12" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B13" s="1"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B14" s="1"/>
+      <c r="C14" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B15" s="1"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B16" s="1"/>
+      <c r="C16" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B18" s="1"/>
+      <c r="C18" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+    </row>
+    <row r="22" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B22" s="1"/>
+      <c r="C22" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="1"/>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+    </row>
+    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B24" s="1"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="1"/>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D26"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
@@ -1649,7 +1846,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1661,7 +1858,7 @@
     <row r="5" spans="2:4" ht="58.5" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" s="14" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1673,83 +1870,83 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="3" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>1</v>
+        <v>64</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
-      <c r="C9" s="3" t="s">
-        <v>41</v>
-      </c>
+      <c r="C9" s="3"/>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
-      <c r="C10" s="3"/>
+      <c r="C10" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
-      <c r="C13" s="3" t="s">
-        <v>52</v>
-      </c>
+      <c r="C13" s="3"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="3"/>
+      <c r="C14" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
-      <c r="C15" s="3" t="s">
-        <v>46</v>
-      </c>
+      <c r="C15" s="3"/>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
-      <c r="C16" s="3"/>
+      <c r="C16" s="3" t="s">
+        <v>69</v>
+      </c>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="1"/>
-      <c r="C17" s="3" t="s">
-        <v>62</v>
-      </c>
+      <c r="C17" s="1"/>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
+      <c r="C18" s="11" t="s">
+        <v>70</v>
+      </c>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:4" ht="59.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B19" s="1"/>
-      <c r="C19" s="3" t="s">
-        <v>66</v>
+      <c r="C19" s="15" t="s">
+        <v>72</v>
       </c>
       <c r="D19" s="1"/>
     </row>
@@ -1792,11 +1989,200 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:D29"/>
+  <sheetViews>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="2.85546875" customWidth="1"/>
+    <col min="3" max="3" width="85.7109375" customWidth="1"/>
+    <col min="4" max="6" width="2.85546875" customWidth="1"/>
+    <col min="7" max="7" width="78.5703125" customWidth="1"/>
+    <col min="8" max="8" width="2.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="1"/>
+      <c r="C3" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B4" s="1"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="2:4" ht="58.5" x14ac:dyDescent="0.25">
+      <c r="B5" s="1"/>
+      <c r="C5" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B7" s="1"/>
+      <c r="C7" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B8" s="1"/>
+      <c r="C8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B9" s="1"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B10" s="1"/>
+      <c r="C10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B11" s="1"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B12" s="1"/>
+      <c r="C12" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B13" s="1"/>
+      <c r="C13" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B14" s="1"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B15" s="1"/>
+      <c r="C15" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B16" s="1"/>
+      <c r="C16" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B17" s="1"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B18" s="1"/>
+      <c r="C18" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B20" s="1"/>
+      <c r="C20" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B21" s="1"/>
+      <c r="C21" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="D21" s="1"/>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+    </row>
+    <row r="23" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+    </row>
+    <row r="25" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B25" s="1"/>
+      <c r="C25" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" s="1"/>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+    </row>
+    <row r="27" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B27" s="1"/>
+      <c r="C27" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="D27" s="1"/>
+    </row>
+    <row r="28" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B28" s="1"/>
+      <c r="C28" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="D28" s="1"/>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
@@ -1817,7 +2203,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>67</v>
+        <v>81</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1826,10 +2212,10 @@
       <c r="C4" s="4"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:4" ht="58.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
-      <c r="C5" s="14" t="s">
-        <v>72</v>
+      <c r="C5" s="2" t="s">
+        <v>84</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1841,83 +2227,83 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="3" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>65</v>
+        <v>34</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
-      <c r="C9" s="3"/>
+      <c r="C9" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
-      <c r="C10" s="3" t="s">
-        <v>42</v>
-      </c>
+      <c r="C10" s="3"/>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
-      <c r="C13" s="3"/>
+      <c r="C13" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="3" t="s">
-        <v>69</v>
-      </c>
+      <c r="C14" s="3"/>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
-      <c r="C15" s="3"/>
+      <c r="C15" s="3" t="s">
+        <v>83</v>
+      </c>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
-      <c r="C16" s="3" t="s">
-        <v>70</v>
-      </c>
+      <c r="C16" s="3"/>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
+      <c r="C17" s="3" t="s">
+        <v>26</v>
+      </c>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
-      <c r="C18" s="11" t="s">
-        <v>71</v>
-      </c>
+      <c r="C18" s="1"/>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:4" ht="59.25" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
-      <c r="C19" s="15" t="s">
-        <v>73</v>
+      <c r="C19" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="D19" s="1"/>
     </row>
@@ -1960,12 +2346,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D33"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2175,438 +2561,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D33"/>
-  <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="2.85546875" customWidth="1"/>
-    <col min="3" max="3" width="85.7109375" customWidth="1"/>
-    <col min="4" max="6" width="2.85546875" customWidth="1"/>
-    <col min="7" max="7" width="78.5703125" customWidth="1"/>
-    <col min="8" max="8" width="2.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="1"/>
-      <c r="C3" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B4" s="1"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B5" s="1"/>
-      <c r="C5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B6" s="1"/>
-      <c r="C6" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B8" s="1"/>
-      <c r="C8" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B9" s="1"/>
-      <c r="C9" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B10" s="1"/>
-      <c r="C10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B11" s="1"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B12" s="1"/>
-      <c r="C12" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B13" s="1"/>
-      <c r="C13" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B14" s="1"/>
-      <c r="C14" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B15" s="1"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="1"/>
-    </row>
-    <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B16" s="1"/>
-      <c r="C16" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B17" s="1"/>
-      <c r="C17" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D17" s="1"/>
-    </row>
-    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B18" s="1"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="1"/>
-    </row>
-    <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B19" s="1"/>
-      <c r="C19" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B20" s="1"/>
-      <c r="C20" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" s="1"/>
-    </row>
-    <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B21" s="1"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B22" s="1"/>
-      <c r="C22" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D22" s="1"/>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-    </row>
-    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B24" s="1"/>
-      <c r="C24" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D24" s="1"/>
-    </row>
-    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B25" s="1"/>
-      <c r="C25" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D25" s="1"/>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-    </row>
-    <row r="27" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B29" s="1"/>
-      <c r="C29" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B31" s="1"/>
-      <c r="C31" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B32" s="1"/>
-      <c r="C32" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="6"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D33"/>
-  <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="2.85546875" customWidth="1"/>
-    <col min="3" max="3" width="85.7109375" customWidth="1"/>
-    <col min="4" max="6" width="2.85546875" customWidth="1"/>
-    <col min="7" max="7" width="78.5703125" customWidth="1"/>
-    <col min="8" max="8" width="2.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="1"/>
-      <c r="C3" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="2:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B4" s="1"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B5" s="1"/>
-      <c r="C5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B6" s="1"/>
-      <c r="C6" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B8" s="1"/>
-      <c r="C8" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B9" s="1"/>
-      <c r="C9" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B10" s="1"/>
-      <c r="C10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B11" s="1"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B12" s="1"/>
-      <c r="C12" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B13" s="1"/>
-      <c r="C13" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B14" s="1"/>
-      <c r="C14" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B15" s="1"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="1"/>
-    </row>
-    <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B16" s="1"/>
-      <c r="C16" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B17" s="1"/>
-      <c r="C17" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D17" s="1"/>
-    </row>
-    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B18" s="1"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="1"/>
-    </row>
-    <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B19" s="1"/>
-      <c r="C19" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B20" s="1"/>
-      <c r="C20" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" s="1"/>
-    </row>
-    <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B21" s="1"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B22" s="1"/>
-      <c r="C22" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D22" s="1"/>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-    </row>
-    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B24" s="1"/>
-      <c r="C24" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D24" s="1"/>
-    </row>
-    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B25" s="1"/>
-      <c r="C25" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D25" s="1"/>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-    </row>
-    <row r="27" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B29" s="1"/>
-      <c r="C29" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B31" s="1"/>
-      <c r="C31" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B32" s="1"/>
-      <c r="C32" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="6"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Added in GrimReaper skills doc 2 new skills.
</commit_message>
<xml_diff>
--- a/GameDesign/Class/6-GrimReaper/Documentation/GrimReaperSkills.xlsx
+++ b/GameDesign/Class/6-GrimReaper/Documentation/GrimReaperSkills.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843" firstSheet="4" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843" firstSheet="4" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="1-ProtectiveWings" sheetId="1" r:id="rId1"/>
@@ -20,8 +20,8 @@
     <sheet name="6-TombStone" sheetId="6" r:id="rId6"/>
     <sheet name="7-MaleficAura" sheetId="7" r:id="rId7"/>
     <sheet name="8-ObscureSoaring" sheetId="8" r:id="rId8"/>
-    <sheet name="Feuil1 (9)" sheetId="9" r:id="rId9"/>
-    <sheet name="Feuil1 (10)" sheetId="10" r:id="rId10"/>
+    <sheet name="9-LivingGround" sheetId="9" r:id="rId9"/>
+    <sheet name="10-SoulReaping" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -33,22 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="86">
-  <si>
-    <t>[[AP: 0 ]]</t>
-  </si>
-  <si>
-    <t>[[MP: 0 ]]</t>
-  </si>
-  <si>
-    <t>[[Range: 0-0 ]]</t>
-  </si>
-  <si>
-    <t>[[Cast in straight line: - ]]</t>
-  </si>
-  <si>
-    <t>[[Modifiable range: - ]]</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="89">
   <si>
     <t>[[Number of casts per turn: - ]]</t>
   </si>
@@ -59,39 +44,9 @@
     <t>[[Max effect accumulation: - ]]</t>
   </si>
   <si>
-    <t>[[Line of sight: - ]]</t>
-  </si>
-  <si>
-    <t>[[Area of effect: - Stright line of 1 cell]]</t>
-  </si>
-  <si>
     <t>Additional Info</t>
   </si>
   <si>
-    <t>[[Damage:  0-0 fire ]]</t>
-  </si>
-  <si>
-    <t>EX: [[Boost taken damage by 10%]] (2 turns)</t>
-  </si>
-  <si>
-    <t>SKILL DESCRIPTION</t>
-  </si>
-  <si>
-    <t>¨¨ ¨¨</t>
-  </si>
-  <si>
-    <t>SKILL NAME</t>
-  </si>
-  <si>
-    <t>Effect name: ''X''.</t>
-  </si>
-  <si>
-    <t>Unbuff ''X'' effect.</t>
-  </si>
-  <si>
-    <t>[[Number of turns between two casts: -  ]]</t>
-  </si>
-  <si>
     <t>Protective Wings</t>
   </si>
   <si>
@@ -291,6 +246,60 @@
   </si>
   <si>
     <t>Teleport the caster at the targeted cell.</t>
+  </si>
+  <si>
+    <t>Living Ground</t>
+  </si>
+  <si>
+    <t>Glyph (2 turns)</t>
+  </si>
+  <si>
+    <t>[[Damage:  40 earth ]]</t>
+  </si>
+  <si>
+    <t>[[Number of turns between two casts: 3 ]]</t>
+  </si>
+  <si>
+    <t>[[Area of effect: - Square of 1 cell ]]</t>
+  </si>
+  <si>
+    <t>[[Range: 0-2 ]]</t>
+  </si>
+  <si>
+    <t>[[Reduce MP by 2]] (1 turn)</t>
+  </si>
+  <si>
+    <t>Inflicts Earth-type damage.                                                              The glyph dealt damage and slow down when an entity start his turn on it.</t>
+  </si>
+  <si>
+    <t>Effect name: ''Slowness''.</t>
+  </si>
+  <si>
+    <t>Soul Reaping</t>
+  </si>
+  <si>
+    <t>Effect name: ''Blinded''.</t>
+  </si>
+  <si>
+    <t>Effect name: ''Invulnerable''.</t>
+  </si>
+  <si>
+    <t>Effect name: ''Heavy''.</t>
+  </si>
+  <si>
+    <t>[[AP: 7 ]]</t>
+  </si>
+  <si>
+    <t>[[Range: 1 ]]</t>
+  </si>
+  <si>
+    <t>[[Damage:  120 Dark ]]</t>
+  </si>
+  <si>
+    <t>If the target is set K/O: [[Caster +7AP]]</t>
+  </si>
+  <si>
+    <t>Inflicts Dark-type damage.                                                                The caster regain the AP used if the damage kill the target.</t>
   </si>
 </sst>
 </file>
@@ -392,7 +401,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -409,9 +418,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -743,10 +749,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D27"/>
+  <dimension ref="B2:D28"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -766,7 +772,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -778,7 +784,7 @@
     <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="2" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -790,21 +796,21 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="3" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
       <c r="C9" s="3" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="D9" s="1"/>
     </row>
@@ -816,7 +822,7 @@
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="3" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="D11" s="1"/>
     </row>
@@ -828,14 +834,14 @@
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
       <c r="C13" s="3" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
       <c r="C14" s="7" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="D14" s="1"/>
     </row>
@@ -847,7 +853,7 @@
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
       <c r="C16" s="3" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="D16" s="1"/>
     </row>
@@ -858,22 +864,22 @@
     </row>
     <row r="18" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B18" s="1"/>
-      <c r="C18" s="11" t="s">
-        <v>27</v>
+      <c r="C18" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B19" s="1"/>
-      <c r="C19" s="11" t="s">
-        <v>28</v>
+      <c r="C19" s="10" t="s">
+        <v>13</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B20" s="1"/>
-      <c r="C20" s="11" t="s">
-        <v>29</v>
+      <c r="C20" s="10" t="s">
+        <v>14</v>
       </c>
       <c r="D20" s="1"/>
     </row>
@@ -891,7 +897,7 @@
     <row r="24" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B24" s="1"/>
       <c r="C24" s="5" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D24" s="1"/>
     </row>
@@ -902,13 +908,22 @@
     </row>
     <row r="26" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B26" s="1"/>
-      <c r="C26" s="10"/>
+      <c r="C26" s="9" t="s">
+        <v>82</v>
+      </c>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="6"/>
+      <c r="C27" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D27" s="1"/>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -918,10 +933,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D33"/>
+  <dimension ref="B2:D24"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -941,7 +956,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>15</v>
+        <v>80</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -950,43 +965,41 @@
       <c r="C4" s="4"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:4" ht="39" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
-      <c r="C5" s="2" t="s">
-        <v>13</v>
+      <c r="C5" s="13" t="s">
+        <v>88</v>
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
-      <c r="C6" s="9" t="s">
-        <v>14</v>
-      </c>
+      <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="C7" s="3" t="s">
+        <v>84</v>
+      </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
-      <c r="C9" s="3" t="s">
-        <v>1</v>
-      </c>
+      <c r="C9" s="3"/>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="3" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D10" s="1"/>
     </row>
@@ -998,134 +1011,73 @@
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
-      <c r="C13" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="C13" s="3"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
       <c r="C14" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B16" s="1"/>
+      <c r="C16" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B17" s="1"/>
+      <c r="C17" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B21" s="1"/>
+      <c r="C21" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B15" s="1"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="1"/>
-    </row>
-    <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B16" s="1"/>
-      <c r="C16" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B17" s="1"/>
-      <c r="C17" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D17" s="1"/>
-    </row>
-    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B18" s="1"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="1"/>
-    </row>
-    <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B19" s="1"/>
-      <c r="C19" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B20" s="1"/>
-      <c r="C20" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" s="1"/>
-    </row>
-    <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B21" s="1"/>
-      <c r="C21" s="3"/>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
-      <c r="C22" s="3" t="s">
-        <v>9</v>
-      </c>
+      <c r="C22" s="1"/>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
+      <c r="C23" s="9"/>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
-      <c r="C24" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D24" s="1"/>
-    </row>
-    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B25" s="1"/>
-      <c r="C25" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D25" s="1"/>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-    </row>
-    <row r="27" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B29" s="1"/>
-      <c r="C29" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B31" s="1"/>
-      <c r="C31" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B32" s="1"/>
-      <c r="C32" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="6"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1158,7 +1110,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1170,7 +1122,7 @@
     <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="2" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1182,21 +1134,21 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="3" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
       <c r="C9" s="3" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="D9" s="1"/>
     </row>
@@ -1208,7 +1160,7 @@
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="3" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="D11" s="1"/>
     </row>
@@ -1220,7 +1172,7 @@
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
       <c r="C13" s="3" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="D13" s="1"/>
     </row>
@@ -1232,7 +1184,7 @@
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
       <c r="C15" s="3" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="D15" s="1"/>
     </row>
@@ -1244,7 +1196,7 @@
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
       <c r="C17" s="3" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="D17" s="1"/>
     </row>
@@ -1262,7 +1214,7 @@
     <row r="21" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B21" s="1"/>
       <c r="C21" s="5" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D21" s="1"/>
     </row>
@@ -1273,7 +1225,9 @@
     </row>
     <row r="23" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B23" s="1"/>
-      <c r="C23" s="10"/>
+      <c r="C23" s="9" t="s">
+        <v>81</v>
+      </c>
       <c r="D23" s="1"/>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
@@ -1312,7 +1266,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1323,8 +1277,8 @@
     </row>
     <row r="5" spans="2:4" ht="39" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
-      <c r="C5" s="12" t="s">
-        <v>39</v>
+      <c r="C5" s="11" t="s">
+        <v>24</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1336,14 +1290,14 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="3" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -1355,21 +1309,21 @@
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="3" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="3" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="D12" s="1"/>
     </row>
@@ -1381,14 +1335,14 @@
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
       <c r="C14" s="3" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
       <c r="C15" s="3" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="D15" s="1"/>
     </row>
@@ -1400,7 +1354,7 @@
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
       <c r="C17" s="3" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="D17" s="1"/>
     </row>
@@ -1411,15 +1365,15 @@
     </row>
     <row r="19" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B19" s="1"/>
-      <c r="C19" s="11" t="s">
-        <v>49</v>
+      <c r="C19" s="10" t="s">
+        <v>34</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B20" s="1"/>
-      <c r="C20" s="11" t="s">
-        <v>48</v>
+      <c r="C20" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="D20" s="1"/>
     </row>
@@ -1437,7 +1391,7 @@
     <row r="24" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B24" s="1"/>
       <c r="C24" s="5" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D24" s="1"/>
     </row>
@@ -1448,7 +1402,7 @@
     </row>
     <row r="26" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B26" s="1"/>
-      <c r="C26" s="10"/>
+      <c r="C26" s="9"/>
       <c r="D26" s="1"/>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
@@ -1467,7 +1421,7 @@
   <dimension ref="B2:D30"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1487,7 +1441,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1498,8 +1452,8 @@
     </row>
     <row r="5" spans="2:4" ht="97.5" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
-      <c r="C5" s="14" t="s">
-        <v>57</v>
+      <c r="C5" s="13" t="s">
+        <v>42</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1511,21 +1465,21 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="3" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
       <c r="C9" s="3" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="D9" s="1"/>
     </row>
@@ -1537,21 +1491,21 @@
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="3" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
       <c r="C13" s="3" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="D13" s="1"/>
     </row>
@@ -1563,7 +1517,7 @@
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
       <c r="C15" s="3" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="D15" s="1"/>
     </row>
@@ -1575,7 +1529,7 @@
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
       <c r="C17" s="3" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="D17" s="1"/>
     </row>
@@ -1586,29 +1540,29 @@
     </row>
     <row r="19" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B19" s="1"/>
-      <c r="C19" s="11" t="s">
-        <v>56</v>
+      <c r="C19" s="10" t="s">
+        <v>41</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B20" s="1"/>
-      <c r="C20" s="11" t="s">
-        <v>58</v>
+      <c r="C20" s="10" t="s">
+        <v>43</v>
       </c>
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B21" s="1"/>
-      <c r="C21" s="11" t="s">
-        <v>60</v>
+      <c r="C21" s="10" t="s">
+        <v>45</v>
       </c>
       <c r="D21" s="1"/>
     </row>
     <row r="22" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B22" s="1"/>
-      <c r="C22" s="11" t="s">
-        <v>59</v>
+      <c r="C22" s="10" t="s">
+        <v>44</v>
       </c>
       <c r="D22" s="1"/>
     </row>
@@ -1626,7 +1580,7 @@
     <row r="26" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B26" s="1"/>
       <c r="C26" s="5" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D26" s="1"/>
     </row>
@@ -1637,15 +1591,15 @@
     </row>
     <row r="28" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B28" s="1"/>
-      <c r="C28" s="13" t="s">
-        <v>54</v>
+      <c r="C28" s="12" t="s">
+        <v>39</v>
       </c>
       <c r="D28" s="1"/>
     </row>
     <row r="29" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B29" s="1"/>
-      <c r="C29" s="13" t="s">
-        <v>55</v>
+      <c r="C29" s="12" t="s">
+        <v>40</v>
       </c>
       <c r="D29" s="1"/>
     </row>
@@ -1685,7 +1639,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1696,8 +1650,8 @@
     </row>
     <row r="5" spans="2:4" ht="58.5" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
-      <c r="C5" s="14" t="s">
-        <v>62</v>
+      <c r="C5" s="13" t="s">
+        <v>47</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1709,14 +1663,14 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="3" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -1728,21 +1682,21 @@
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="3" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="3" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="D12" s="1"/>
     </row>
@@ -1754,7 +1708,7 @@
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
       <c r="C14" s="3" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="D14" s="1"/>
     </row>
@@ -1766,7 +1720,7 @@
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
       <c r="C16" s="3" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="D16" s="1"/>
     </row>
@@ -1778,7 +1732,7 @@
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
       <c r="C18" s="3" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="D18" s="1"/>
     </row>
@@ -1796,7 +1750,7 @@
     <row r="22" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B22" s="1"/>
       <c r="C22" s="5" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D22" s="1"/>
     </row>
@@ -1807,7 +1761,7 @@
     </row>
     <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B24" s="1"/>
-      <c r="C24" s="10"/>
+      <c r="C24" s="9"/>
       <c r="D24" s="1"/>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
@@ -1846,7 +1800,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1857,8 +1811,8 @@
     </row>
     <row r="5" spans="2:4" ht="58.5" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
-      <c r="C5" s="14" t="s">
-        <v>71</v>
+      <c r="C5" s="13" t="s">
+        <v>56</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1870,14 +1824,14 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="3" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -1889,21 +1843,21 @@
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="3" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="3" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="D12" s="1"/>
     </row>
@@ -1915,7 +1869,7 @@
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
       <c r="C14" s="3" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="D14" s="1"/>
     </row>
@@ -1927,7 +1881,7 @@
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
       <c r="C16" s="3" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="D16" s="1"/>
     </row>
@@ -1938,15 +1892,15 @@
     </row>
     <row r="18" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B18" s="1"/>
-      <c r="C18" s="11" t="s">
-        <v>70</v>
+      <c r="C18" s="10" t="s">
+        <v>55</v>
       </c>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:4" ht="59.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B19" s="1"/>
-      <c r="C19" s="15" t="s">
-        <v>72</v>
+      <c r="C19" s="14" t="s">
+        <v>57</v>
       </c>
       <c r="D19" s="1"/>
     </row>
@@ -1964,7 +1918,7 @@
     <row r="23" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B23" s="1"/>
       <c r="C23" s="5" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D23" s="1"/>
     </row>
@@ -1975,7 +1929,7 @@
     </row>
     <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B25" s="1"/>
-      <c r="C25" s="10"/>
+      <c r="C25" s="9"/>
       <c r="D25" s="1"/>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
@@ -2014,7 +1968,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -2025,8 +1979,8 @@
     </row>
     <row r="5" spans="2:4" ht="58.5" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
-      <c r="C5" s="14" t="s">
-        <v>80</v>
+      <c r="C5" s="13" t="s">
+        <v>65</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -2038,14 +1992,14 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="3" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -2057,7 +2011,7 @@
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="3" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="D10" s="1"/>
     </row>
@@ -2069,14 +2023,14 @@
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
       <c r="C13" s="7" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D13" s="1"/>
     </row>
@@ -2088,14 +2042,14 @@
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
       <c r="C15" s="3" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
       <c r="C16" s="3" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D16" s="1"/>
     </row>
@@ -2107,7 +2061,7 @@
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
       <c r="C18" s="3" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="D18" s="1"/>
     </row>
@@ -2118,15 +2072,15 @@
     </row>
     <row r="20" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B20" s="1"/>
-      <c r="C20" s="11" t="s">
-        <v>76</v>
+      <c r="C20" s="10" t="s">
+        <v>61</v>
       </c>
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B21" s="1"/>
-      <c r="C21" s="11" t="s">
-        <v>77</v>
+      <c r="C21" s="10" t="s">
+        <v>62</v>
       </c>
       <c r="D21" s="1"/>
     </row>
@@ -2144,7 +2098,7 @@
     <row r="25" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B25" s="1"/>
       <c r="C25" s="5" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D25" s="1"/>
     </row>
@@ -2155,15 +2109,15 @@
     </row>
     <row r="27" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B27" s="1"/>
-      <c r="C27" s="10" t="s">
-        <v>78</v>
+      <c r="C27" s="9" t="s">
+        <v>63</v>
       </c>
       <c r="D27" s="1"/>
     </row>
     <row r="28" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B28" s="1"/>
-      <c r="C28" s="10" t="s">
-        <v>79</v>
+      <c r="C28" s="9" t="s">
+        <v>64</v>
       </c>
       <c r="D28" s="1"/>
     </row>
@@ -2203,7 +2157,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -2215,7 +2169,7 @@
     <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="2" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -2227,21 +2181,21 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="3" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
       <c r="C9" s="3" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="D9" s="1"/>
     </row>
@@ -2253,21 +2207,21 @@
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="3" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
       <c r="C13" s="3" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="D13" s="1"/>
     </row>
@@ -2279,7 +2233,7 @@
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
       <c r="C15" s="3" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="D15" s="1"/>
     </row>
@@ -2291,7 +2245,7 @@
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
       <c r="C17" s="3" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="D17" s="1"/>
     </row>
@@ -2303,7 +2257,7 @@
     <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
       <c r="C19" s="3" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="D19" s="1"/>
     </row>
@@ -2321,7 +2275,7 @@
     <row r="23" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B23" s="1"/>
       <c r="C23" s="5" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D23" s="1"/>
     </row>
@@ -2332,7 +2286,7 @@
     </row>
     <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B25" s="1"/>
-      <c r="C25" s="10"/>
+      <c r="C25" s="9"/>
       <c r="D25" s="1"/>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
@@ -2348,10 +2302,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D33"/>
+  <dimension ref="B2:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2371,7 +2325,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="8" t="s">
-        <v>15</v>
+        <v>71</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -2380,138 +2334,130 @@
       <c r="C4" s="4"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:4" ht="58.5" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
-      <c r="C5" s="2" t="s">
-        <v>13</v>
+      <c r="C5" s="13" t="s">
+        <v>78</v>
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
-      <c r="C6" s="9" t="s">
-        <v>14</v>
-      </c>
+      <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="C7" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
       <c r="C9" s="3" t="s">
-        <v>1</v>
+        <v>76</v>
       </c>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
-      <c r="C10" s="3" t="s">
-        <v>2</v>
-      </c>
+      <c r="C10" s="3"/>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
-      <c r="C11" s="3"/>
+      <c r="C11" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="3" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
       <c r="C13" s="3" t="s">
-        <v>8</v>
+        <v>37</v>
       </c>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="C14" s="3"/>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
-      <c r="C15" s="3"/>
+      <c r="C15" s="3" t="s">
+        <v>74</v>
+      </c>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
-      <c r="C16" s="3" t="s">
-        <v>18</v>
-      </c>
+      <c r="C16" s="3"/>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
-      <c r="C17" s="7" t="s">
-        <v>7</v>
+      <c r="C17" s="3" t="s">
+        <v>75</v>
       </c>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="1"/>
-      <c r="C18" s="3"/>
+      <c r="C18" s="1"/>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B19" s="1"/>
-      <c r="C19" s="3" t="s">
-        <v>5</v>
+      <c r="C19" s="10" t="s">
+        <v>73</v>
       </c>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B20" s="1"/>
-      <c r="C20" s="3" t="s">
-        <v>6</v>
+      <c r="C20" s="10" t="s">
+        <v>77</v>
       </c>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B21" s="1"/>
-      <c r="C21" s="3"/>
+      <c r="C21" s="10" t="s">
+        <v>72</v>
+      </c>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
-      <c r="C22" s="3" t="s">
-        <v>9</v>
-      </c>
+      <c r="C22" s="1"/>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-    </row>
-    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="23" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
-      <c r="C24" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="C24" s="1"/>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B25" s="1"/>
-      <c r="C25" s="3" t="s">
-        <v>12</v>
+      <c r="C25" s="5" t="s">
+        <v>3</v>
       </c>
       <c r="D25" s="1"/>
     </row>
@@ -2520,42 +2466,17 @@
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B27" s="1"/>
+      <c r="C27" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="D27" s="1"/>
+    </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B29" s="1"/>
-      <c r="C29" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B31" s="1"/>
-      <c r="C31" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B32" s="1"/>
-      <c r="C32" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="6"/>
+      <c r="D28" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>